<commit_message>
Updates from WRI on 11/7 with data updates.
</commit_message>
<xml_diff>
--- a/InputData/add-outputs/SCoHIbP/Social Cost of Health Impacts by Pollutant_HK.xlsx
+++ b/InputData/add-outputs/SCoHIbP/Social Cost of Health Impacts by Pollutant_HK.xlsx
@@ -11547,8 +11547,8 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="文档" ma:contentTypeID="0x01010095990DC6317597479C114DD4E6AB1F33" ma:contentTypeVersion="14" ma:contentTypeDescription="新建文档。" ma:contentTypeScope="" ma:versionID="40ddae6b2e673ca4350ee4f9e73461e0">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="7889d872-e2a2-4afb-87bc-97561eced75f" xmlns:ns3="c9df191c-55f2-496b-9838-9a5abe4742ad" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7e116a0b9e2b9814d46da3cedae238ac" ns1:_="" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010095990DC6317597479C114DD4E6AB1F33" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="00c0eb7d4c43453177323eb1ac58d7e7">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="7889d872-e2a2-4afb-87bc-97561eced75f" xmlns:ns3="c9df191c-55f2-496b-9838-9a5abe4742ad" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b5fe72540fcc493259a136614ad94e00" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="7889d872-e2a2-4afb-87bc-97561eced75f"/>
     <xsd:import namespace="c9df191c-55f2-496b-9838-9a5abe4742ad"/>
@@ -11582,12 +11582,12 @@
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="http://schemas.microsoft.com/sharepoint/v3" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="18" nillable="true" ma:displayName="统一合规性策略属性" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
+    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="18" nillable="true" ma:displayName="Unified Compliance Policy Properties" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="19" nillable="true" ma:displayName="统一合规性策略 UI 操作" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
+    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="19" nillable="true" ma:displayName="Unified Compliance Policy UI Action" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
@@ -11596,7 +11596,7 @@
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="7889d872-e2a2-4afb-87bc-97561eced75f" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="8" nillable="true" ma:displayName="共享对象:" ma:description="" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="8" nillable="true" ma:displayName="Shared With" ma:description="" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -11615,7 +11615,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="9" nillable="true" ma:displayName="共享对象详细信息" ma:description="" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="9" nillable="true" ma:displayName="Shared With Details" ma:description="" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -11690,8 +11690,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="内容类型"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="标题"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -11798,7 +11798,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD6EBB9A-A7C8-42E5-A078-918B2B11D0AE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6A3BF07-7ED7-416F-97DE-E942FDD976CB}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>